<commit_message>
Listados casi listos del 15 de agosto
</commit_message>
<xml_diff>
--- a/Agosto/17 agosto/mexicali/PLANTILLA_MONITORES_17 AGOSTO 2024.xlsx
+++ b/Agosto/17 agosto/mexicali/PLANTILLA_MONITORES_17 AGOSTO 2024.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tecnm\Documents\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proyecto01TICs\Documents\Evaluatec2024\Agosto\17 agosto\mexicali\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7B26B6-D63D-4EEB-B237-EBF284930980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MONITORES" sheetId="1" r:id="rId1"/>
@@ -19,17 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -133,7 +123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -348,7 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -357,44 +347,43 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -657,18 +646,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" name="NÚMERO DE EMPLEADO" dataDxfId="9"/>
-    <tableColumn id="2" name="CORREO" dataDxfId="8"/>
-    <tableColumn id="3" name="CURP" dataDxfId="7"/>
-    <tableColumn id="4" name="NOMBRE COMPLETO (SIN FORMULAS)" dataDxfId="6"/>
-    <tableColumn id="5" name="DEPARTAMENTO DE ADSCRIPCIÓN" dataDxfId="5"/>
-    <tableColumn id="8" name="FECHA OFICIAL MONITOREO" dataDxfId="4"/>
-    <tableColumn id="9" name="HORORARIO PARA MONITOREAR EN EL OFICIAL" dataDxfId="3"/>
-    <tableColumn id="10" name="VERSIÓN DE EXAMEN" dataDxfId="2"/>
-    <tableColumn id="11" name="Columna1" dataDxfId="1"/>
-    <tableColumn id="12" name="Columna2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NÚMERO DE EMPLEADO" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="CORREO" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="CURP" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="NOMBRE COMPLETO (SIN FORMULAS)" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="DEPARTAMENTO DE ADSCRIPCIÓN" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="FECHA OFICIAL MONITOREO" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="HORORARIO PARA MONITOREAR EN EL OFICIAL" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="VERSIÓN DE EXAMEN" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Columna1" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Columna2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -970,11 +959,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,16 +981,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>22</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -1010,175 +999,175 @@
       <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="26" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>959</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="5"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="5"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="5"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="2"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -1735,9 +1724,9 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2" display="mailto:nieves@itmexicali.edu.mx"/>
-    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="mailto:nieves@itmexicali.edu.mx" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>